<commit_message>
Automation for CSP 1.16 Script issue fixed
</commit_message>
<xml_diff>
--- a/resources/excels/NG.xlsx
+++ b/resources/excels/NG.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2394650\IdeaProjects\cs-portal-automation_selenium1\resources\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\23127836\IdeaProjects\cs-portal-automation_selenium\resources\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="35205" windowHeight="10425" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="35205" windowHeight="10425" firstSheet="11" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="1385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3017" uniqueCount="1385">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -4204,7 +4204,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -4495,7 +4495,7 @@
         <xdr:cNvPr id="2" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4543,7 +4543,7 @@
         <xdr:cNvPr id="3" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5208,8 +5208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -5297,9 +5297,6 @@
       </c>
       <c r="I2" s="21" t="s">
         <v>1232</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>1233</v>
       </c>
     </row>
   </sheetData>
@@ -5941,7 +5938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>

</xml_diff>